<commit_message>
Actualización general de presupuestos y archivos
</commit_message>
<xml_diff>
--- a/nuevos_afiliados.xlsx
+++ b/nuevos_afiliados.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6115d10aab34be5f/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Diego Mauricio\Desktop\Lina marcela\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6ADEA40C-62CF-4039-B02C-AF480B562883}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03FAA912-CF09-4984-97F5-4C0E6AED82DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{23414C93-14AC-4765-928B-1938BE4A86AD}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{23414C93-14AC-4765-928B-1938BE4A86AD}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -183,13 +183,13 @@
     <t>Miembro</t>
   </si>
   <si>
-    <t>Empresa</t>
-  </si>
-  <si>
     <t>Categoria</t>
   </si>
   <si>
-    <t>afiliados</t>
+    <t>Compañía</t>
+  </si>
+  <si>
+    <t>Tipo_Afiliado</t>
   </si>
 </sst>
 </file>
@@ -315,9 +315,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - Tema de 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -355,7 +355,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -461,7 +461,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -603,7 +603,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -614,27 +614,28 @@
   <dimension ref="A1:C35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C26"/>
+      <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="18" customWidth="1"/>
-    <col min="2" max="2" width="17.85546875" customWidth="1"/>
+    <col min="2" max="2" width="17.88671875" customWidth="1"/>
+    <col min="3" max="3" width="12.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>49</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>50</v>
       </c>
       <c r="C1" s="6" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -645,7 +646,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="22.5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -656,7 +657,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="22.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -667,7 +668,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
@@ -678,7 +679,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
@@ -689,7 +690,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
@@ -700,7 +701,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="22.5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
@@ -711,7 +712,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="22.5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>11</v>
       </c>
@@ -722,7 +723,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>13</v>
       </c>
@@ -733,7 +734,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="22.5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>15</v>
       </c>
@@ -744,7 +745,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="33.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>16</v>
       </c>
@@ -755,7 +756,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>17</v>
       </c>
@@ -766,7 +767,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>18</v>
       </c>
@@ -777,7 +778,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>19</v>
       </c>
@@ -788,7 +789,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="22.5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>20</v>
       </c>
@@ -799,7 +800,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>22</v>
       </c>
@@ -810,7 +811,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="22.5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>24</v>
       </c>
@@ -821,7 +822,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>25</v>
       </c>
@@ -832,7 +833,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="22.5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>26</v>
       </c>
@@ -843,7 +844,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="22.5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>27</v>
       </c>
@@ -854,7 +855,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="22.5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>28</v>
       </c>
@@ -865,7 +866,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="22.5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>30</v>
       </c>
@@ -876,7 +877,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>31</v>
       </c>
@@ -887,7 +888,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="22.5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>32</v>
       </c>
@@ -898,7 +899,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>33</v>
       </c>
@@ -909,7 +910,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="22.5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>34</v>
       </c>
@@ -920,7 +921,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>36</v>
       </c>
@@ -931,7 +932,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="22.5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>38</v>
       </c>
@@ -942,7 +943,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>39</v>
       </c>
@@ -953,7 +954,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="33.75" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>40</v>
       </c>
@@ -964,7 +965,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="22.5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>41</v>
       </c>
@@ -975,7 +976,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>42</v>
       </c>
@@ -986,7 +987,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" s="3" t="s">
         <v>44</v>
       </c>
@@ -997,7 +998,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="22.5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>45</v>
       </c>
@@ -1010,5 +1011,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>